<commit_message>
Wing update docs 11/28/17
</commit_message>
<xml_diff>
--- a/Wing results/2017_10_16Lab 18 prelim data table.xlsx
+++ b/Wing results/2017_10_16Lab 18 prelim data table.xlsx
@@ -2698,9 +2698,6 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2708,6 +2705,9 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3024,7 +3024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J45"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
+    <sheetView topLeftCell="B8" workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
@@ -3035,14 +3035,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="5" t="s">
         <v>866</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
+      <c r="H2" s="5"/>
+      <c r="I2" s="5" t="s">
         <v>863</v>
       </c>
-      <c r="J2" s="1"/>
+      <c r="J2" s="5"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.45">
       <c r="C3" t="s">
@@ -28564,7 +28564,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -28580,20 +28580,20 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>869</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A4" s="2"/>
+      <c r="A4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>870</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A6" s="2"/>
+      <c r="A6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
@@ -28711,19 +28711,19 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>3.3450190886210597E-11</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>1.6583896045681699E-10</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>2.0113149096296E-7</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>7.24713940929324E-6</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="3">
         <v>9.0647013483970601E-5</v>
       </c>
       <c r="G12" t="s">
@@ -28734,19 +28734,19 @@
       <c r="A13" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>1.37188564472613E-17</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>5.6895774940944203E-17</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <v>1.46080396724549E-12</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <v>2.00937127202869E-10</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="3">
         <v>1.15691384258361E-8</v>
       </c>
       <c r="G13">
@@ -28754,21 +28754,21 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>869</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A16" s="2"/>
+      <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>870</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A18" s="2"/>
-      <c r="I18" s="3"/>
+      <c r="A18" s="1"/>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
@@ -28789,7 +28789,7 @@
       <c r="F19" t="s">
         <v>5</v>
       </c>
-      <c r="I19" s="3"/>
+      <c r="I19" s="2"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
@@ -28813,7 +28813,7 @@
       <c r="G20" t="s">
         <v>873</v>
       </c>
-      <c r="I20" s="3"/>
+      <c r="I20" s="2"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
@@ -28837,19 +28837,19 @@
       <c r="G21" t="s">
         <v>873</v>
       </c>
-      <c r="I21" s="3"/>
+      <c r="I21" s="2"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="4">
         <v>1.2402583248297501E-2</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="4">
         <v>3.69865395084511E-2</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="4">
         <v>0.413144768818834</v>
       </c>
       <c r="E22" t="s">
@@ -28861,22 +28861,22 @@
       <c r="G22" t="s">
         <v>873</v>
       </c>
-      <c r="I22" s="3"/>
+      <c r="I22" s="2"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="4">
         <v>4.1742607629697602E-3</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="4">
         <v>1.33476705457184E-2</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="4">
         <v>0.213994160699118</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="4">
         <v>0.64914740938093796</v>
       </c>
       <c r="F23" t="s">
@@ -28885,49 +28885,49 @@
       <c r="G23" t="s">
         <v>873</v>
       </c>
-      <c r="I23" s="3"/>
+      <c r="I23" s="2"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="3">
         <v>1.5928662326767001E-12</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="3">
         <v>7.8970933550865199E-12</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="3">
         <v>9.5776900458552207E-9</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="3">
         <v>3.4510187663301098E-7</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F24" s="3">
         <v>4.3165244516176496E-6</v>
       </c>
       <c r="G24" t="s">
         <v>873</v>
       </c>
-      <c r="I24" s="3"/>
+      <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="3">
         <v>6.53278878441014E-19</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="3">
         <v>2.7093226162354401E-18</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="3">
         <v>6.9562093678356706E-14</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="3">
         <v>9.5684346287080496E-12</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F25" s="3">
         <v>5.5091135361124404E-10</v>
       </c>
       <c r="G25">
@@ -28935,10 +28935,10 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A26" s="2"/>
+      <c r="A26" s="1"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="2" t="s">
         <v>872</v>
       </c>
     </row>

</xml_diff>